<commit_message>
Fix for issue XLSReader tends to convert long number to scientific notation #1
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\Development\Personal\SearchBot\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\Development\Personal\Processor\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="13125"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="28800" windowHeight="13125"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>"Test"</t>
+  </si>
+  <si>
+    <t>gagag</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +547,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>123456789012345</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>